<commit_message>
create TestC and test suit for it
It is used to run TestC according to my operation,and it will use the data from user and password to test if the result will show us the user page which consists of "Product" and "Carts" menus.
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsfile/data.xlsx
+++ b/src/main/resources/xlsfile/data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{051219B1-B53D-464D-A3D3-CFBC5461FEAC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324F3BAB-306E-400B-B09D-8E524A6C90DE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="3" r:id="rId1"/>
@@ -43,133 +43,134 @@
     <t>hello</t>
   </si>
   <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>imageLocation</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>p0001</t>
+  </si>
+  <si>
+    <t>p0002</t>
+  </si>
+  <si>
+    <t>p0003</t>
+  </si>
+  <si>
+    <t>p0004</t>
+  </si>
+  <si>
+    <t>p0005</t>
+  </si>
+  <si>
+    <t>garden.jpg</t>
+  </si>
+  <si>
+    <t>banana.jpg</t>
+  </si>
+  <si>
+    <t>orange.jpg</t>
+  </si>
+  <si>
+    <t>papaya.jpg</t>
+  </si>
+  <si>
+    <t>rambutan.jpg</t>
+  </si>
+  <si>
+    <t>Garden</t>
+  </si>
+  <si>
+    <t>Banana</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Papaya</t>
+  </si>
+  <si>
+    <t>Rambutan</t>
+  </si>
+  <si>
+    <t>The garden which you can grow everything on earth</t>
+  </si>
+  <si>
+    <t>A good fruit with very cheap price</t>
+  </si>
+  <si>
+    <t>Nothing good about it</t>
+  </si>
+  <si>
+    <t>Use for papaya salad</t>
+  </si>
+  <si>
+    <t>An expensive fruit from the sout</t>
+  </si>
+  <si>
+    <t>transactionId</t>
+  </si>
+  <si>
+    <t>ProductId</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>t001</t>
+  </si>
+  <si>
+    <t>t002</t>
+  </si>
+  <si>
+    <t>t003</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>t004</t>
+  </si>
+  <si>
+    <t>t005</t>
+  </si>
+  <si>
+    <t>t006</t>
+  </si>
+  <si>
+    <t>SaleOrderId</t>
+  </si>
+  <si>
+    <t>SaleTransactoin</t>
+  </si>
+  <si>
+    <t>o001</t>
+  </si>
+  <si>
+    <t>o002</t>
+  </si>
+  <si>
+    <t>t001,t002</t>
+  </si>
+  <si>
+    <t>p0006</t>
+  </si>
+  <si>
+    <t>Unknow</t>
+  </si>
+  <si>
+    <t>Don't use this</t>
+  </si>
+  <si>
+    <t>t003,t004,t005,t006</t>
+  </si>
+  <si>
     <t>productId</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>imageLocation</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t>p0001</t>
-  </si>
-  <si>
-    <t>p0002</t>
-  </si>
-  <si>
-    <t>p0003</t>
-  </si>
-  <si>
-    <t>p0004</t>
-  </si>
-  <si>
-    <t>p0005</t>
-  </si>
-  <si>
-    <t>garden.jpg</t>
-  </si>
-  <si>
-    <t>banana.jpg</t>
-  </si>
-  <si>
-    <t>orange.jpg</t>
-  </si>
-  <si>
-    <t>papaya.jpg</t>
-  </si>
-  <si>
-    <t>rambutan.jpg</t>
-  </si>
-  <si>
-    <t>Garden</t>
-  </si>
-  <si>
-    <t>Banana</t>
-  </si>
-  <si>
-    <t>Orange</t>
-  </si>
-  <si>
-    <t>Papaya</t>
-  </si>
-  <si>
-    <t>Rambutan</t>
-  </si>
-  <si>
-    <t>The garden which you can grow everything on earth</t>
-  </si>
-  <si>
-    <t>A good fruit with very cheap price</t>
-  </si>
-  <si>
-    <t>Nothing good about it</t>
-  </si>
-  <si>
-    <t>Use for papaya salad</t>
-  </si>
-  <si>
-    <t>An expensive fruit from the sout</t>
-  </si>
-  <si>
-    <t>transactionId</t>
-  </si>
-  <si>
-    <t>ProductId</t>
-  </si>
-  <si>
-    <t>amount</t>
-  </si>
-  <si>
-    <t>t001</t>
-  </si>
-  <si>
-    <t>t002</t>
-  </si>
-  <si>
-    <t>t003</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>t004</t>
-  </si>
-  <si>
-    <t>t005</t>
-  </si>
-  <si>
-    <t>t006</t>
-  </si>
-  <si>
-    <t>SaleOrderId</t>
-  </si>
-  <si>
-    <t>SaleTransactoin</t>
-  </si>
-  <si>
-    <t>o001</t>
-  </si>
-  <si>
-    <t>o002</t>
-  </si>
-  <si>
-    <t>t001,t002</t>
-  </si>
-  <si>
-    <t>p0006</t>
-  </si>
-  <si>
-    <t>Unknow</t>
-  </si>
-  <si>
-    <t>Don't use this</t>
-  </si>
-  <si>
-    <t>t003,t004,t005,t006</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -177,21 +178,28 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -214,15 +222,15 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -277,7 +285,7 @@
     <tableColumn id="2" xr3:uid="{85BFE5BF-A718-4639-B784-3A9E3DF9453C}" name="name"/>
     <tableColumn id="3" xr3:uid="{658925E2-0413-49B0-ADC4-9893E7094EBE}" name="description"/>
     <tableColumn id="4" xr3:uid="{19E76E9F-2D9C-4924-B711-72CEAB2874EB}" name="imageLocation"/>
-    <tableColumn id="5" xr3:uid="{CCA0166F-DFB0-427F-9264-7796610873AF}" name="price" dataDxfId="0" dataCellStyle="Comma"/>
+    <tableColumn id="5" xr3:uid="{CCA0166F-DFB0-427F-9264-7796610873AF}" name="price" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -564,13 +572,13 @@
       <selection activeCell="B2" sqref="B2:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -581,7 +589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -592,7 +600,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -603,7 +611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -615,6 +623,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -627,140 +636,141 @@
   <dimension ref="B2:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="B2" sqref="B2:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.625" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" s="1">
         <v>20000</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" s="1">
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="1">
         <v>280</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F6" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F7" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
         <v>45</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>46</v>
       </c>
-      <c r="D8" t="s">
-        <v>47</v>
-      </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F8" s="1">
         <v>-1</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -772,94 +782,95 @@
   <dimension ref="B2:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B2" sqref="B2:D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.625" customWidth="1"/>
+    <col min="3" max="3" width="11.625" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>31</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8">
         <v>6</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -872,39 +883,40 @@
   <dimension ref="B2:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
         <v>40</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
         <v>42</v>
       </c>
-      <c r="C3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>43</v>
-      </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>